<commit_message>
Se cierra bucle infinito para que cuando no exista la palabra vuelva a pedir otra palabra
</commit_message>
<xml_diff>
--- a/archivos/sopa_entendimiento.xlsx
+++ b/archivos/sopa_entendimiento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Config\MIPSasm\archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4310528-25D2-42CD-9700-615EC9E5127E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFF2CFB-80AD-40A7-886A-24EC2B9CF8C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>h</t>
   </si>
@@ -60,9 +60,6 @@
     <t>y</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>\r o \0</t>
   </si>
   <si>
@@ -82,13 +79,37 @@
   </si>
   <si>
     <t>asi</t>
+  </si>
+  <si>
+    <t>ccaracteres + cccaracteres-1 + 2</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>filas</t>
+  </si>
+  <si>
+    <t>columnas</t>
+  </si>
+  <si>
+    <t>vertical</t>
+  </si>
+  <si>
+    <t>100 + 99 + 2 = 201</t>
+  </si>
+  <si>
+    <t>\n</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,8 +131,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,6 +155,11 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -154,12 +187,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -174,10 +208,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="40% - Accent3" xfId="2" builtinId="39"/>
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -456,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:Q11"/>
+  <dimension ref="B1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -468,12 +506,12 @@
     <col min="16" max="16" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:19" x14ac:dyDescent="0.3">
       <c r="E1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
       <c r="E2">
         <v>0</v>
       </c>
@@ -502,21 +540,21 @@
         <v>8</v>
       </c>
       <c r="P2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="2:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="L3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
@@ -548,7 +586,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -573,14 +611,20 @@
       <c r="K5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="6">
         <v>13</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="6">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="O5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -590,8 +634,11 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="P6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
       <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
@@ -622,8 +669,20 @@
       <c r="M7" s="4">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="P7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R7" t="s">
+        <v>3</v>
+      </c>
+      <c r="S7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>1</v>
       </c>
@@ -643,16 +702,16 @@
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L8" s="2">
+        <v>9</v>
+      </c>
+      <c r="L8" s="6">
         <v>13</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -663,7 +722,7 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
       <c r="D10" s="1" t="s">
         <v>5</v>
       </c>
@@ -695,7 +754,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>2</v>
       </c>
@@ -703,11 +762,11 @@
         <v>4</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2" t="s">
@@ -715,13 +774,38 @@
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" s="2">
+        <v>15</v>
+      </c>
+      <c r="L11" s="6">
         <v>0</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11" s="6">
         <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="K15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15">
+        <v>100</v>
+      </c>
+      <c r="N15" t="s">
+        <v>21</v>
+      </c>
+      <c r="O15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="K16" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="N16" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>